<commit_message>
Add ServiceLocator,merge RunAVL and RunBST to RunTree
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Id</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>SBS</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -377,14 +380,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -440,6 +444,57 @@
         <v>43159</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>51503002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>55</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>51503003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>43159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>51503004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>43159</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>